<commit_message>
adding csv and updated modal
</commit_message>
<xml_diff>
--- a/JS_cup_calculations.xlsx
+++ b/JS_cup_calculations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acnah\Documents\AppAcademy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acnah\Documents\AppAcademy\Javascript_project_12_27_21\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{66B3842B-BAC7-40AE-90C7-55038CF9E5B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78CD04F9-E819-4081-B875-EB32B4AEC764}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6531F925-A851-456B-AE83-4BE61E84895D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{6531F925-A851-456B-AE83-4BE61E84895D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
   <si>
     <t>alcohol type</t>
   </si>
@@ -63,6 +63,36 @@
   </si>
   <si>
     <t>in solo cups</t>
+  </si>
+  <si>
+    <t>standard drink size (oz)</t>
+  </si>
+  <si>
+    <t>standard drink size (L)</t>
+  </si>
+  <si>
+    <t>full red cup (oz)</t>
+  </si>
+  <si>
+    <t>full red cup (L)</t>
+  </si>
+  <si>
+    <t>pure alcohol per standard drink (L)</t>
+  </si>
+  <si>
+    <t>Pure Alcohol (L)</t>
+  </si>
+  <si>
+    <t>number of red cup standard drinks</t>
+  </si>
+  <si>
+    <t>number of full cup drinks</t>
+  </si>
+  <si>
+    <t>pure alcohol per full cup (L)</t>
+  </si>
+  <si>
+    <t>pure Alcohol (oz)</t>
   </si>
 </sst>
 </file>
@@ -418,8 +448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F2CBC8C-8173-453F-AF25-7CECF7622DBB}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -522,12 +552,212 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{236151D2-82B3-471F-8481-5EC020E83AF7}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.88671875" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" customWidth="1"/>
+    <col min="6" max="6" width="16.88671875" customWidth="1"/>
+    <col min="7" max="7" width="30.109375" customWidth="1"/>
+    <col min="8" max="8" width="25.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="C2">
+        <v>12</v>
+      </c>
+      <c r="D2">
+        <f>C2/33.814</f>
+        <v>0.35488259300881292</v>
+      </c>
+      <c r="E2">
+        <v>16</v>
+      </c>
+      <c r="F2">
+        <f>E2/33.814</f>
+        <v>0.47317679067841723</v>
+      </c>
+      <c r="G2">
+        <f>D2 * B2</f>
+        <v>1.7744129650440647E-2</v>
+      </c>
+      <c r="H2">
+        <f>F2 *B2</f>
+        <v>2.3658839533920863E-2</v>
+      </c>
+      <c r="K2">
+        <f xml:space="preserve"> 0.01774413 * 33.814</f>
+        <v>0.60000001181999996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D4" si="0">C3/33.814</f>
+        <v>0.14786774708700537</v>
+      </c>
+      <c r="E3">
+        <v>16</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F4" si="1">E3/33.814</f>
+        <v>0.47317679067841723</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G4" si="2">D3 * B3</f>
+        <v>1.7744129650440643E-2</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H4" si="3">F3 *B3</f>
+        <v>5.6781214881410066E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="C4">
+        <v>1.5</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>4.4360324126101615E-2</v>
+      </c>
+      <c r="E4">
+        <v>16</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>0.47317679067841723</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="2"/>
+        <v>1.7744129650440647E-2</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="3"/>
+        <v>0.18927071627136691</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>3.6</v>
+      </c>
+      <c r="F8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8">
+        <f>A8/G2</f>
+        <v>202.88399999999999</v>
+      </c>
+      <c r="H8">
+        <f>A8/H2</f>
+        <v>152.16299999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F9" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9">
+        <f>A8/G3</f>
+        <v>202.88400000000004</v>
+      </c>
+      <c r="H9">
+        <f>A8/H3</f>
+        <v>63.401250000000005</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F10" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10">
+        <f>A8/G4</f>
+        <v>202.88399999999999</v>
+      </c>
+      <c r="H10">
+        <f>A8/H4</f>
+        <v>19.020374999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <f>A8 * 33.814</f>
+        <v>121.7304</v>
+      </c>
+      <c r="G15">
+        <f xml:space="preserve"> A15/K2</f>
+        <v>202.8839960031853</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>